<commit_message>
Added more test cases
</commit_message>
<xml_diff>
--- a/Test cases and bugs.xlsx
+++ b/Test cases and bugs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gagel_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Aptana_Workspace\AppAggregator\AppAggregator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Test cases</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>newly approved apps show up in search and under all apps</t>
+  </si>
+  <si>
+    <t>Searched apps show up in search box</t>
+  </si>
+  <si>
+    <t>new users receive confirmation email</t>
+  </si>
+  <si>
+    <t>Admins can view a page to view newly submitted apps</t>
   </si>
 </sst>
 </file>
@@ -416,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,25 +503,61 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug with approval again, added more links, added tests
</commit_message>
<xml_diff>
--- a/Test cases and bugs.xlsx
+++ b/Test cases and bugs.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Aptana_Workspace\AppAggregator\AppAggregator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Test cases</t>
   </si>
@@ -84,13 +79,19 @@
   </si>
   <si>
     <t>Admins can view a page to view newly submitted apps</t>
+  </si>
+  <si>
+    <t>All users can see all approved apps</t>
+  </si>
+  <si>
+    <t>Moderators and admins can delete comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -417,21 +418,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="79.28515625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -439,7 +440,7 @@
     <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="45" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,12 +454,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="36" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -472,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -486,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -494,12 +495,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="50.25" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -507,7 +508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -515,7 +516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -523,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -531,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -539,7 +540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -547,7 +548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -555,9 +556,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>